<commit_message>
adding send email subprocess
</commit_message>
<xml_diff>
--- a/EssilorLuxottica Projects/LUX - 7.1 - Process GL Report/Data/Config.xlsx
+++ b/EssilorLuxottica Projects/LUX - 7.1 - Process GL Report/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.1 - Process GL Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C618696F-9EC0-4A44-A100-37ACC661E0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE7350F-30FD-4756-B75A-B7F6C540A427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -310,6 +310,30 @@
   </si>
   <si>
     <t>\\LRRBTUIPFSP100\Profiles\Uipath_26\Desktop\EssilorLuxottica Projects\LUX-7.1_Daily Fallout Report\LUX - 7.1 - Process Fallout Reports\Data\Input\Fallout Application</t>
+  </si>
+  <si>
+    <t>strToEmailAddress</t>
+  </si>
+  <si>
+    <t>strEmailPort</t>
+  </si>
+  <si>
+    <t>strEmailServer</t>
+  </si>
+  <si>
+    <t>strCCEmailAddress</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.1_EmailPort</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.1_ToEmailAddress</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.1_EmailServer</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.1_CCEmailAddress</t>
   </si>
 </sst>
 </file>
@@ -374,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -385,6 +409,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -703,7 +728,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -3181,8 +3206,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3224,10 +3249,38 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4225,5 +4278,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>